<commit_message>
fixed migrations and cancel bid and updated burndown
</commit_message>
<xml_diff>
--- a/docs/Planning/Sprint3Burndown.xlsx
+++ b/docs/Planning/Sprint3Burndown.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\webDevProject\3MusketeersAndARifleman\docs\Planning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{34CD140E-62CC-4149-934A-AAA5EA340013}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0E2CD51-9979-4857-8CC2-F9D7123E9D79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{5BD6E5F6-9D7D-46B9-9C3C-C2EEC4B0C5B4}"/>
   </bookViews>
@@ -542,6 +542,9 @@
                 <c:pt idx="2">
                   <c:v>44648</c:v>
                 </c:pt>
+                <c:pt idx="3">
+                  <c:v>44650</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -559,6 +562,9 @@
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>17</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -617,6 +623,9 @@
                 <c:pt idx="2">
                   <c:v>44648</c:v>
                 </c:pt>
+                <c:pt idx="3">
+                  <c:v>44650</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -631,6 +640,9 @@
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>32</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1861,7 +1873,7 @@
   <dimension ref="A1:P24"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="O13" sqref="O13"/>
+      <selection activeCell="P6" sqref="P6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2034,7 +2046,9 @@
       <c r="O5" s="2">
         <v>26</v>
       </c>
-      <c r="P5" s="2"/>
+      <c r="P5" s="2">
+        <v>32</v>
+      </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A6" s="6">
@@ -2066,8 +2080,12 @@
       </c>
       <c r="K6" s="1"/>
       <c r="L6" s="1"/>
-      <c r="N6" s="21"/>
-      <c r="O6" s="2"/>
+      <c r="N6" s="21">
+        <v>44650</v>
+      </c>
+      <c r="O6" s="2">
+        <v>17</v>
+      </c>
       <c r="P6" s="2"/>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
added in tests and updated burndown
</commit_message>
<xml_diff>
--- a/docs/Planning/Sprint3Burndown.xlsx
+++ b/docs/Planning/Sprint3Burndown.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\webDevProject\3MusketeersAndARifleman\docs\Planning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0E2CD51-9979-4857-8CC2-F9D7123E9D79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D711EAA6-DF62-43D2-A4ED-E51139096741}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{5BD6E5F6-9D7D-46B9-9C3C-C2EEC4B0C5B4}"/>
   </bookViews>
@@ -36,22 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="13">
-  <si>
-    <t>backlog items by Thursday, Feb 24th</t>
-  </si>
-  <si>
-    <t>backlog items by Tuesday, March 1st</t>
-  </si>
-  <si>
-    <t>backlog items by Thursday, March 3rd</t>
-  </si>
-  <si>
-    <t>actual</t>
-  </si>
-  <si>
-    <t>estimated</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>Estimated</t>
   </si>
@@ -60,21 +45,6 @@
   </si>
   <si>
     <t>total estimated task hours</t>
-  </si>
-  <si>
-    <t>Sprint 1</t>
-  </si>
-  <si>
-    <t>(rollover) 60</t>
-  </si>
-  <si>
-    <t>(rollover) 62</t>
-  </si>
-  <si>
-    <t>(rollover) 72</t>
-  </si>
-  <si>
-    <t>(rollover) 42</t>
   </si>
 </sst>
 </file>
@@ -545,6 +515,9 @@
                 <c:pt idx="3">
                   <c:v>44650</c:v>
                 </c:pt>
+                <c:pt idx="4">
+                  <c:v>44651</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -565,6 +538,9 @@
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -626,6 +602,9 @@
                 <c:pt idx="3">
                   <c:v>44650</c:v>
                 </c:pt>
+                <c:pt idx="4">
+                  <c:v>44651</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -643,6 +622,12 @@
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1873,7 +1858,7 @@
   <dimension ref="A1:P24"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="P6" sqref="P6"/>
+      <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1894,78 +1879,42 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="29.4" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A1" s="19" t="s">
-        <v>8</v>
-      </c>
+      <c r="A1" s="19"/>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A2" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="F2" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="G2" s="3" t="s">
+      <c r="A2" s="3"/>
+      <c r="B2" s="4"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="10"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="4"/>
+      <c r="I2" s="5"/>
+      <c r="K2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="H2" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="I2" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>7</v>
-      </c>
       <c r="L2" s="2">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="N2" s="2"/>
       <c r="O2" s="2" t="s">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="P2" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A3" s="6">
-        <v>54</v>
-      </c>
-      <c r="B3" s="2">
-        <v>2</v>
-      </c>
-      <c r="C3" s="7">
         <v>1</v>
       </c>
-      <c r="D3" s="6">
-        <v>68</v>
-      </c>
-      <c r="E3" s="2">
-        <v>2</v>
-      </c>
-      <c r="F3" s="11">
-        <v>3</v>
-      </c>
-      <c r="G3" s="22" t="s">
-        <v>10</v>
-      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A3" s="6"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="11"/>
+      <c r="G3" s="22"/>
       <c r="H3" s="2"/>
-      <c r="I3" s="7">
-        <v>0</v>
-      </c>
+      <c r="I3" s="7"/>
       <c r="N3" s="21">
         <v>44642</v>
       </c>
@@ -1977,29 +1926,15 @@
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A4" s="6">
-        <v>57</v>
-      </c>
-      <c r="B4" s="2">
-        <v>2</v>
-      </c>
-      <c r="C4" s="7">
-        <v>1</v>
-      </c>
-      <c r="D4" s="22" t="s">
-        <v>9</v>
-      </c>
+      <c r="A4" s="6"/>
+      <c r="B4" s="2"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="22"/>
       <c r="E4" s="2"/>
-      <c r="F4" s="11">
-        <v>3</v>
-      </c>
-      <c r="G4" s="22" t="s">
-        <v>11</v>
-      </c>
+      <c r="F4" s="11"/>
+      <c r="G4" s="22"/>
       <c r="H4" s="2"/>
-      <c r="I4" s="7">
-        <v>2</v>
-      </c>
+      <c r="I4" s="7"/>
       <c r="K4" s="1"/>
       <c r="L4" s="1"/>
       <c r="N4" s="21">
@@ -2013,31 +1948,15 @@
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A5" s="6">
-        <v>63</v>
-      </c>
-      <c r="B5" s="2">
-        <v>2</v>
-      </c>
-      <c r="C5" s="7">
-        <v>2</v>
-      </c>
-      <c r="D5" s="22" t="s">
-        <v>10</v>
-      </c>
+      <c r="A5" s="6"/>
+      <c r="B5" s="2"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="22"/>
       <c r="E5" s="2"/>
-      <c r="F5" s="11">
-        <v>0</v>
-      </c>
-      <c r="G5" s="22">
-        <v>51</v>
-      </c>
-      <c r="H5" s="2">
-        <v>1</v>
-      </c>
-      <c r="I5" s="7">
-        <v>1</v>
-      </c>
+      <c r="F5" s="11"/>
+      <c r="G5" s="22"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="7"/>
       <c r="K5" s="1"/>
       <c r="L5" s="1"/>
       <c r="N5" s="21">
@@ -2051,33 +1970,15 @@
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A6" s="6">
-        <v>58</v>
-      </c>
-      <c r="B6" s="2">
-        <v>2</v>
-      </c>
-      <c r="C6" s="7">
-        <v>2</v>
-      </c>
-      <c r="D6" s="6">
-        <v>56</v>
-      </c>
-      <c r="E6" s="2">
-        <v>1</v>
-      </c>
-      <c r="F6" s="11">
-        <v>1</v>
-      </c>
-      <c r="G6" s="22">
-        <v>49</v>
-      </c>
-      <c r="H6" s="2">
-        <v>2</v>
-      </c>
-      <c r="I6" s="7">
-        <v>0</v>
-      </c>
+      <c r="A6" s="6"/>
+      <c r="B6" s="2"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="11"/>
+      <c r="G6" s="22"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="7"/>
       <c r="K6" s="1"/>
       <c r="L6" s="1"/>
       <c r="N6" s="21">
@@ -2086,59 +1987,39 @@
       <c r="O6" s="2">
         <v>17</v>
       </c>
-      <c r="P6" s="2"/>
+      <c r="P6" s="2">
+        <v>17</v>
+      </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A7" s="6">
-        <v>55</v>
+      <c r="A7" s="6"/>
+      <c r="B7" s="2"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="11"/>
+      <c r="G7" s="22"/>
+      <c r="H7" s="2"/>
+      <c r="I7" s="7"/>
+      <c r="K7" s="18"/>
+      <c r="L7" s="1"/>
+      <c r="N7" s="21">
+        <v>44651</v>
       </c>
-      <c r="B7" s="2">
-        <v>2</v>
-      </c>
-      <c r="C7" s="7">
-        <v>2</v>
-      </c>
-      <c r="D7" s="6">
-        <v>72</v>
-      </c>
-      <c r="E7" s="2">
-        <v>3</v>
-      </c>
-      <c r="F7" s="11">
+      <c r="O7" s="2">
         <v>0</v>
       </c>
-      <c r="G7" s="22" t="s">
-        <v>12</v>
-      </c>
-      <c r="H7" s="2"/>
-      <c r="I7" s="7">
+      <c r="P7" s="2">
         <v>0</v>
       </c>
-      <c r="K7" s="18"/>
-      <c r="L7" s="1"/>
-      <c r="N7" s="21"/>
-      <c r="O7" s="2"/>
-      <c r="P7" s="2"/>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A8" s="6">
-        <v>53</v>
-      </c>
-      <c r="B8" s="2">
-        <v>2</v>
-      </c>
-      <c r="C8" s="7">
-        <v>3</v>
-      </c>
-      <c r="D8" s="6">
-        <v>42</v>
-      </c>
-      <c r="E8" s="2">
-        <v>2</v>
-      </c>
-      <c r="F8" s="11">
-        <v>0</v>
-      </c>
+      <c r="A8" s="6"/>
+      <c r="B8" s="2"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="11"/>
       <c r="G8" s="22"/>
       <c r="H8" s="2"/>
       <c r="I8" s="7"/>
@@ -2146,24 +2027,12 @@
       <c r="L8" s="1"/>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A9" s="6">
-        <v>62</v>
-      </c>
-      <c r="B9" s="2">
-        <v>4</v>
-      </c>
-      <c r="C9" s="7">
-        <v>0</v>
-      </c>
-      <c r="D9" s="6">
-        <v>59</v>
-      </c>
-      <c r="E9" s="2">
-        <v>2</v>
-      </c>
-      <c r="F9" s="11">
-        <v>2</v>
-      </c>
+      <c r="A9" s="6"/>
+      <c r="B9" s="2"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="11"/>
       <c r="G9" s="6"/>
       <c r="H9" s="2"/>
       <c r="I9" s="7"/>
@@ -2171,24 +2040,12 @@
       <c r="L9" s="1"/>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A10" s="6">
-        <v>60</v>
-      </c>
-      <c r="B10" s="2">
-        <v>2</v>
-      </c>
-      <c r="C10" s="7">
-        <v>0</v>
-      </c>
-      <c r="D10" s="6">
-        <v>50</v>
-      </c>
-      <c r="E10" s="2">
-        <v>2</v>
-      </c>
-      <c r="F10" s="11">
-        <v>1</v>
-      </c>
+      <c r="A10" s="6"/>
+      <c r="B10" s="2"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="11"/>
       <c r="G10" s="6"/>
       <c r="H10" s="2"/>
       <c r="I10" s="7"/>
@@ -2199,15 +2056,9 @@
       <c r="A11" s="12"/>
       <c r="B11" s="13"/>
       <c r="C11" s="14"/>
-      <c r="D11" s="12">
-        <v>52</v>
-      </c>
-      <c r="E11" s="13">
-        <v>1</v>
-      </c>
-      <c r="F11" s="15">
-        <v>1</v>
-      </c>
+      <c r="D11" s="12"/>
+      <c r="E11" s="13"/>
+      <c r="F11" s="15"/>
       <c r="G11" s="12"/>
       <c r="H11" s="13"/>
       <c r="I11" s="14"/>
@@ -2216,32 +2067,14 @@
     </row>
     <row r="12" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="8"/>
-      <c r="B12" s="9">
-        <f>SUM(B3:B10)</f>
-        <v>18</v>
-      </c>
-      <c r="C12" s="16">
-        <f>SUM(C3:C10)</f>
-        <v>11</v>
-      </c>
+      <c r="B12" s="9"/>
+      <c r="C12" s="16"/>
       <c r="D12" s="8"/>
-      <c r="E12" s="9">
-        <f>SUM(E3:E11)</f>
-        <v>13</v>
-      </c>
-      <c r="F12" s="17">
-        <f>SUM(F3:F11)</f>
-        <v>11</v>
-      </c>
+      <c r="E12" s="9"/>
+      <c r="F12" s="17"/>
       <c r="G12" s="8"/>
-      <c r="H12" s="9">
-        <f>SUM(H3:H11)</f>
-        <v>3</v>
-      </c>
-      <c r="I12" s="16">
-        <f>SUM(I3:I11)</f>
-        <v>3</v>
-      </c>
+      <c r="H12" s="9"/>
+      <c r="I12" s="16"/>
       <c r="K12" s="1"/>
       <c r="L12" s="1"/>
     </row>

</xml_diff>